<commit_message>
IFB only stocks trade value in Hemat
</commit_message>
<xml_diff>
--- a/Karmozd-sum.xlsx
+++ b/Karmozd-sum.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahdi/Dropbox/GitHub/karmozd-sum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A6AA66-F25C-6C43-A851-62D33D94793A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B577567-8721-1A4B-AED9-E712159596D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-960" yWindow="-20120" windowWidth="28040" windowHeight="16140" activeTab="1" xr2:uid="{4DEE318E-4C7C-6A44-B197-2FC704C7AD9D}"/>
+    <workbookView xWindow="-960" yWindow="-20120" windowWidth="28040" windowHeight="16140" activeTab="2" xr2:uid="{4DEE318E-4C7C-6A44-B197-2FC704C7AD9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
     <sheet name="IFB-Monthly" sheetId="1" r:id="rId2"/>
-    <sheet name="TSE" sheetId="2" r:id="rId3"/>
+    <sheet name="IFB-Annual" sheetId="4" r:id="rId3"/>
+    <sheet name="TSE" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="810">
   <si>
     <t>1400-01</t>
   </si>
@@ -2449,6 +2450,24 @@
   </si>
   <si>
     <t>1401-04</t>
+  </si>
+  <si>
+    <t>JYear</t>
+  </si>
+  <si>
+    <t>1397-</t>
+  </si>
+  <si>
+    <t>1398-</t>
+  </si>
+  <si>
+    <t>1399-</t>
+  </si>
+  <si>
+    <t>1400-</t>
+  </si>
+  <si>
+    <t>IFB-Stocks-TradeValue(Hemat)</t>
   </si>
 </sst>
 </file>
@@ -2461,7 +2480,7 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2510,6 +2529,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2534,7 +2560,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2552,6 +2578,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma 3 2" xfId="3" xr:uid="{27E8BF95-53D4-9040-9FF4-DF4CF9BF5330}"/>
@@ -2872,7 +2899,7 @@
   <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2998,12 +3025,12 @@
       <c r="B3" s="6">
         <v>862.03550938666331</v>
       </c>
-      <c r="C3" s="6">
-        <v>4665.5044118442684</v>
+      <c r="C3">
+        <v>327.4981722</v>
       </c>
       <c r="D3" s="6">
         <f>C3+B3</f>
-        <v>5527.5399212309312</v>
+        <v>1189.5336815866633</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -3016,46 +3043,46 @@
       </c>
       <c r="L3" s="7">
         <f>$D3 * K3</f>
-        <v>33.607442721084062</v>
+        <v>7.2323647840469132</v>
       </c>
       <c r="M3" s="4">
         <v>5.1200000000000004E-3</v>
       </c>
       <c r="N3" s="7">
         <f>$D3 * M3</f>
-        <v>28.301004396702371</v>
+        <v>6.0904124497237166</v>
       </c>
       <c r="O3" s="4">
         <v>2.4000000000000001E-4</v>
       </c>
       <c r="P3" s="7">
         <f>$D3 * O3</f>
-        <v>1.3266095810954235</v>
+        <v>0.28548808358079919</v>
       </c>
       <c r="Q3" s="4">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="R3" s="7">
         <f>$D3 * Q3</f>
-        <v>1.1055079842461863</v>
+        <v>0.23790673631733267</v>
       </c>
       <c r="S3" s="4">
         <v>4.8000000000000001E-4</v>
       </c>
       <c r="T3" s="5">
         <f>$D3 * S3</f>
-        <v>2.653219162190847</v>
+        <v>0.57097616716159838</v>
       </c>
       <c r="U3" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="V3" s="7">
         <f>$D3 * U3</f>
-        <v>27.637699606154655</v>
+        <v>5.9476684079333166</v>
       </c>
       <c r="W3" s="7">
         <f>SUM(L3,N3,P3,R3,T3,V3)</f>
-        <v>94.631483451473557</v>
+        <v>20.364816628763677</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
@@ -3065,12 +3092,12 @@
       <c r="B4" s="6">
         <v>2425.46162105553</v>
       </c>
-      <c r="C4" s="6">
-        <v>1771.5475146458086</v>
+      <c r="C4">
+        <v>939.17679384479595</v>
       </c>
       <c r="D4" s="6">
         <f t="shared" ref="D4:D5" si="0">C4+B4</f>
-        <v>4197.0091357013389</v>
+        <v>3364.6384149003261</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6">
@@ -3091,46 +3118,46 @@
       </c>
       <c r="L4" s="7">
         <f t="shared" ref="L4:L5" si="1">$D4 * K4</f>
-        <v>25.517815545064142</v>
+        <v>20.457001562593984</v>
       </c>
       <c r="M4" s="4">
         <v>5.1200000000000004E-3</v>
       </c>
       <c r="N4" s="7">
         <f t="shared" ref="N4:N5" si="2">$D4 * M4</f>
-        <v>21.488686774790857</v>
+        <v>17.22694868428967</v>
       </c>
       <c r="O4" s="4">
         <v>2.4000000000000001E-4</v>
       </c>
       <c r="P4" s="7">
         <f t="shared" ref="P4:P5" si="3">$D4 * O4</f>
-        <v>1.0072821925683213</v>
+        <v>0.80751321957607824</v>
       </c>
       <c r="Q4" s="4">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="R4" s="7">
         <f t="shared" ref="R4:R5" si="4">$D4 * Q4</f>
-        <v>0.83940182714026779</v>
+        <v>0.67292768298006522</v>
       </c>
       <c r="S4" s="4">
         <v>4.8000000000000001E-4</v>
       </c>
       <c r="T4" s="5">
         <f t="shared" ref="T4:T5" si="5">$D4 * S4</f>
-        <v>2.0145643851366426</v>
+        <v>1.6150264391521565</v>
       </c>
       <c r="U4" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="V4" s="7">
         <f t="shared" ref="V4:V5" si="6">$D4 * U4</f>
-        <v>20.985045678506694</v>
+        <v>16.82319207450163</v>
       </c>
       <c r="W4" s="7">
         <f t="shared" ref="W4:W5" si="7">SUM(L4,N4,P4,R4,T4,V4)</f>
-        <v>71.852796403206924</v>
+        <v>57.602609663093588</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
@@ -3140,12 +3167,12 @@
       <c r="B5" s="6">
         <v>466.36133860917471</v>
       </c>
-      <c r="C5" s="6">
-        <v>324.19709658733541</v>
+      <c r="C5">
+        <v>214.38297593607513</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" si="0"/>
-        <v>790.55843519651012</v>
+        <v>680.74431454524984</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6">
@@ -3166,46 +3193,46 @@
       </c>
       <c r="L5" s="7">
         <f t="shared" si="1"/>
-        <v>4.8065952859947814</v>
+        <v>4.1389254324351192</v>
       </c>
       <c r="M5" s="4">
         <v>5.1200000000000004E-3</v>
       </c>
       <c r="N5" s="7">
         <f t="shared" si="2"/>
-        <v>4.0476591882061319</v>
+        <v>3.4854108904716794</v>
       </c>
       <c r="O5" s="4">
         <v>2.4000000000000001E-4</v>
       </c>
       <c r="P5" s="7">
         <f t="shared" si="3"/>
-        <v>0.18973402444716242</v>
+        <v>0.16337863549085996</v>
       </c>
       <c r="Q5" s="4">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="R5" s="7">
         <f t="shared" si="4"/>
-        <v>0.15811168703930203</v>
+        <v>0.13614886290904998</v>
       </c>
       <c r="S5" s="4">
         <v>4.8000000000000001E-4</v>
       </c>
       <c r="T5" s="5">
         <f t="shared" si="5"/>
-        <v>0.37946804889432484</v>
+        <v>0.32675727098171992</v>
       </c>
       <c r="U5" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="V5" s="7">
         <f t="shared" si="6"/>
-        <v>3.9527921759825508</v>
+        <v>3.4037215727262491</v>
       </c>
       <c r="W5" s="7">
         <f t="shared" si="7"/>
-        <v>13.534360410564254</v>
+        <v>11.654342665014678</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
@@ -3301,14 +3328,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70668EB9-07E2-2143-8D2A-6657005E9699}">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -3742,6 +3769,83 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF03B052-F2D4-A246-ADFB-9FAC6344CC60}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>804</v>
+      </c>
+      <c r="B1" t="s">
+        <v>787</v>
+      </c>
+      <c r="C1" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>808</v>
+      </c>
+      <c r="B2" s="9">
+        <v>3274981.7220000001</v>
+      </c>
+      <c r="C2">
+        <v>327.4981722</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>807</v>
+      </c>
+      <c r="B3">
+        <v>9391767.9384479597</v>
+      </c>
+      <c r="C3">
+        <v>939.17679384479595</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>806</v>
+      </c>
+      <c r="B4">
+        <v>2143829.7593607511</v>
+      </c>
+      <c r="C4">
+        <v>214.38297593607513</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>805</v>
+      </c>
+      <c r="B5">
+        <v>458576.76494457602</v>
+      </c>
+      <c r="C5">
+        <v>45.8576764944576</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B5">
+    <sortCondition descending="1" ref="A2:A5"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{356E6000-CEE8-D247-91E0-0A0DA47010B7}">
   <dimension ref="A1:E722"/>
   <sheetViews>

</xml_diff>